<commit_message>
Variant,ourworldindata,monkeypox notebooks, and figures
</commit_message>
<xml_diff>
--- a/WHO/WHO_COVID_Excess_Deaths_EstimatesByIncome.xlsx
+++ b/WHO/WHO_COVID_Excess_Deaths_EstimatesByIncome.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/naritas_who_int/Documents/HQ DDI/COVID GEM/Data/Public release - May 2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rucdk-my.sharepoint.com/personal/mannov_ruc_dk/Documents/Pandemix/Github/PandemiX/WHO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{7908F12D-416D-4488-8351-4900754FC095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A875EAE-6E82-4B31-BD4B-14BD991DE533}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{7908F12D-416D-4488-8351-4900754FC095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95EB8139-004F-43A2-898B-B88D5312D78E}"/>
   <bookViews>
-    <workbookView xWindow="18765" yWindow="-12720" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="7" r:id="rId1"/>
@@ -487,6 +487,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -522,24 +540,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -902,7 +902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE0C47D-8CC1-413A-8398-F2E357B72927}">
   <dimension ref="B4:L11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
@@ -917,76 +917,76 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="86.25" customHeight="1" thickBot="1">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="24"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="30"/>
     </row>
     <row r="6" spans="2:12">
       <c r="B6" s="6"/>
       <c r="L6" s="7"/>
     </row>
     <row r="7" spans="2:12" ht="47.25" customHeight="1">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="27"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="33"/>
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="8"/>
       <c r="L8" s="7"/>
     </row>
     <row r="9" spans="2:12" ht="230.25" customHeight="1">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="30"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="36"/>
     </row>
     <row r="10" spans="2:12">
       <c r="B10" s="6"/>
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="2:12" ht="48" customHeight="1">
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="33"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1009,7 +1009,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
@@ -4213,7 +4213,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B534207-8CE0-4F97-B144-A62F7A6AE306}">
   <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
@@ -4222,7 +4224,7 @@
     <col min="3" max="3" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="34" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="22" customWidth="1"/>
     <col min="7" max="9" width="14.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="3" customWidth="1"/>
     <col min="11" max="16384" width="11.42578125" style="3"/>
@@ -4346,7 +4348,7 @@
       <c r="E12" s="9">
         <v>203977974</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="23" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="9">
@@ -4375,7 +4377,7 @@
       <c r="E13" s="10">
         <v>65843490</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="10">
@@ -4404,7 +4406,7 @@
       <c r="E14" s="10">
         <v>26801643</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G14" s="10">
@@ -4433,7 +4435,7 @@
       <c r="E15" s="10">
         <v>18136805</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="10">
@@ -4462,7 +4464,7 @@
       <c r="E16" s="10">
         <v>11261450</v>
       </c>
-      <c r="F16" s="36" t="s">
+      <c r="F16" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G16" s="10">
@@ -4491,7 +4493,7 @@
       <c r="E17" s="10">
         <v>5813135</v>
       </c>
-      <c r="F17" s="36" t="s">
+      <c r="F17" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="10">
@@ -4520,7 +4522,7 @@
       <c r="E18" s="10">
         <v>1743203</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G18" s="10">
@@ -4549,7 +4551,7 @@
       <c r="E19" s="11">
         <v>208309683</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="F19" s="25" t="s">
         <v>10</v>
       </c>
       <c r="G19" s="11">
@@ -4578,7 +4580,7 @@
       <c r="E20" s="12">
         <v>65386472</v>
       </c>
-      <c r="F20" s="38" t="s">
+      <c r="F20" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="12">
@@ -4607,7 +4609,7 @@
       <c r="E21" s="12">
         <v>25950764</v>
       </c>
-      <c r="F21" s="38" t="s">
+      <c r="F21" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="12">
@@ -4636,7 +4638,7 @@
       <c r="E22" s="12">
         <v>16735763</v>
       </c>
-      <c r="F22" s="38" t="s">
+      <c r="F22" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="12">
@@ -4665,7 +4667,7 @@
       <c r="E23" s="12">
         <v>9740786</v>
       </c>
-      <c r="F23" s="38" t="s">
+      <c r="F23" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G23" s="12">
@@ -4694,7 +4696,7 @@
       <c r="E24" s="12">
         <v>4381209</v>
       </c>
-      <c r="F24" s="38" t="s">
+      <c r="F24" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G24" s="12">
@@ -4723,7 +4725,7 @@
       <c r="E25" s="13">
         <v>1066658</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="27" t="s">
         <v>10</v>
       </c>
       <c r="G25" s="13">
@@ -4752,7 +4754,7 @@
       <c r="E26" s="9">
         <v>208445941</v>
       </c>
-      <c r="F26" s="35" t="s">
+      <c r="F26" s="23" t="s">
         <v>10</v>
       </c>
       <c r="G26" s="9">
@@ -4781,7 +4783,7 @@
       <c r="E27" s="10">
         <v>68124322</v>
       </c>
-      <c r="F27" s="36" t="s">
+      <c r="F27" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G27" s="10">
@@ -4810,7 +4812,7 @@
       <c r="E28" s="10">
         <v>27729035</v>
       </c>
-      <c r="F28" s="36" t="s">
+      <c r="F28" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G28" s="10">
@@ -4839,7 +4841,7 @@
       <c r="E29" s="10">
         <v>18742260</v>
       </c>
-      <c r="F29" s="36" t="s">
+      <c r="F29" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G29" s="10">
@@ -4868,7 +4870,7 @@
       <c r="E30" s="10">
         <v>11627425</v>
       </c>
-      <c r="F30" s="36" t="s">
+      <c r="F30" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G30" s="10">
@@ -4897,7 +4899,7 @@
       <c r="E31" s="10">
         <v>5941427</v>
       </c>
-      <c r="F31" s="36" t="s">
+      <c r="F31" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G31" s="10">
@@ -4926,7 +4928,7 @@
       <c r="E32" s="10">
         <v>1861763</v>
       </c>
-      <c r="F32" s="36" t="s">
+      <c r="F32" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G32" s="10">
@@ -4955,7 +4957,7 @@
       <c r="E33" s="11">
         <v>212910494</v>
       </c>
-      <c r="F33" s="37" t="s">
+      <c r="F33" s="25" t="s">
         <v>10</v>
       </c>
       <c r="G33" s="11">
@@ -4984,7 +4986,7 @@
       <c r="E34" s="12">
         <v>67746944</v>
       </c>
-      <c r="F34" s="38" t="s">
+      <c r="F34" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G34" s="12">
@@ -5013,7 +5015,7 @@
       <c r="E35" s="12">
         <v>26824358</v>
       </c>
-      <c r="F35" s="38" t="s">
+      <c r="F35" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G35" s="12">
@@ -5042,7 +5044,7 @@
       <c r="E36" s="12">
         <v>17339446</v>
       </c>
-      <c r="F36" s="38" t="s">
+      <c r="F36" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G36" s="12">
@@ -5071,7 +5073,7 @@
       <c r="E37" s="12">
         <v>10061079</v>
       </c>
-      <c r="F37" s="38" t="s">
+      <c r="F37" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G37" s="12">
@@ -5100,7 +5102,7 @@
       <c r="E38" s="12">
         <v>4501886</v>
       </c>
-      <c r="F38" s="38" t="s">
+      <c r="F38" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G38" s="12">
@@ -5129,7 +5131,7 @@
       <c r="E39" s="13">
         <v>1149936</v>
       </c>
-      <c r="F39" s="39" t="s">
+      <c r="F39" s="27" t="s">
         <v>10</v>
       </c>
       <c r="G39" s="13">
@@ -5158,7 +5160,7 @@
       <c r="E40" s="9">
         <v>762087503</v>
       </c>
-      <c r="F40" s="35" t="s">
+      <c r="F40" s="23" t="s">
         <v>10</v>
       </c>
       <c r="G40" s="9">
@@ -5187,7 +5189,7 @@
       <c r="E41" s="10">
         <v>378598490</v>
       </c>
-      <c r="F41" s="36" t="s">
+      <c r="F41" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G41" s="10">
@@ -5216,7 +5218,7 @@
       <c r="E42" s="10">
         <v>191275477</v>
       </c>
-      <c r="F42" s="36" t="s">
+      <c r="F42" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G42" s="10">
@@ -5245,7 +5247,7 @@
       <c r="E43" s="10">
         <v>143324929</v>
       </c>
-      <c r="F43" s="36" t="s">
+      <c r="F43" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G43" s="10">
@@ -5274,7 +5276,7 @@
       <c r="E44" s="10">
         <v>94516981</v>
       </c>
-      <c r="F44" s="36" t="s">
+      <c r="F44" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G44" s="10">
@@ -5303,7 +5305,7 @@
       <c r="E45" s="10">
         <v>45403597</v>
       </c>
-      <c r="F45" s="36" t="s">
+      <c r="F45" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G45" s="10">
@@ -5332,7 +5334,7 @@
       <c r="E46" s="10">
         <v>17412724</v>
       </c>
-      <c r="F46" s="36" t="s">
+      <c r="F46" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G46" s="10">
@@ -5361,7 +5363,7 @@
       <c r="E47" s="11">
         <v>815666334</v>
       </c>
-      <c r="F47" s="37" t="s">
+      <c r="F47" s="25" t="s">
         <v>10</v>
       </c>
       <c r="G47" s="11">
@@ -5390,7 +5392,7 @@
       <c r="E48" s="12">
         <v>395247660</v>
       </c>
-      <c r="F48" s="38" t="s">
+      <c r="F48" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G48" s="12">
@@ -5419,7 +5421,7 @@
       <c r="E49" s="12">
         <v>194968778</v>
       </c>
-      <c r="F49" s="38" t="s">
+      <c r="F49" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G49" s="12">
@@ -5448,7 +5450,7 @@
       <c r="E50" s="12">
         <v>143448976</v>
       </c>
-      <c r="F50" s="38" t="s">
+      <c r="F50" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G50" s="12">
@@ -5477,7 +5479,7 @@
       <c r="E51" s="12">
         <v>90913956</v>
       </c>
-      <c r="F51" s="38" t="s">
+      <c r="F51" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G51" s="12">
@@ -5506,7 +5508,7 @@
       <c r="E52" s="12">
         <v>38815558</v>
       </c>
-      <c r="F52" s="38" t="s">
+      <c r="F52" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G52" s="12">
@@ -5535,7 +5537,7 @@
       <c r="E53" s="13">
         <v>12431371</v>
       </c>
-      <c r="F53" s="39" t="s">
+      <c r="F53" s="27" t="s">
         <v>10</v>
       </c>
       <c r="G53" s="13">
@@ -5564,7 +5566,7 @@
       <c r="E54" s="9">
         <v>766401685</v>
       </c>
-      <c r="F54" s="35" t="s">
+      <c r="F54" s="23" t="s">
         <v>10</v>
       </c>
       <c r="G54" s="9">
@@ -5593,7 +5595,7 @@
       <c r="E55" s="10">
         <v>382667853</v>
       </c>
-      <c r="F55" s="36" t="s">
+      <c r="F55" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G55" s="10">
@@ -5622,7 +5624,7 @@
       <c r="E56" s="10">
         <v>196018824</v>
       </c>
-      <c r="F56" s="36" t="s">
+      <c r="F56" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G56" s="10">
@@ -5651,7 +5653,7 @@
       <c r="E57" s="10">
         <v>146574361</v>
       </c>
-      <c r="F57" s="36" t="s">
+      <c r="F57" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G57" s="10">
@@ -5680,7 +5682,7 @@
       <c r="E58" s="10">
         <v>97670708</v>
       </c>
-      <c r="F58" s="36" t="s">
+      <c r="F58" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G58" s="10">
@@ -5709,7 +5711,7 @@
       <c r="E59" s="10">
         <v>47068773</v>
       </c>
-      <c r="F59" s="36" t="s">
+      <c r="F59" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G59" s="10">
@@ -5738,7 +5740,7 @@
       <c r="E60" s="10">
         <v>18266763</v>
       </c>
-      <c r="F60" s="36" t="s">
+      <c r="F60" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G60" s="10">
@@ -5767,7 +5769,7 @@
       <c r="E61" s="11">
         <v>820093590</v>
       </c>
-      <c r="F61" s="37" t="s">
+      <c r="F61" s="25" t="s">
         <v>10</v>
       </c>
       <c r="G61" s="11">
@@ -5796,7 +5798,7 @@
       <c r="E62" s="12">
         <v>400207558</v>
       </c>
-      <c r="F62" s="38" t="s">
+      <c r="F62" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G62" s="12">
@@ -5825,7 +5827,7 @@
       <c r="E63" s="12">
         <v>199799299</v>
       </c>
-      <c r="F63" s="38" t="s">
+      <c r="F63" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G63" s="12">
@@ -5854,7 +5856,7 @@
       <c r="E64" s="12">
         <v>146519633</v>
       </c>
-      <c r="F64" s="38" t="s">
+      <c r="F64" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G64" s="12">
@@ -5883,7 +5885,7 @@
       <c r="E65" s="12">
         <v>93879303</v>
       </c>
-      <c r="F65" s="38" t="s">
+      <c r="F65" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G65" s="12">
@@ -5912,7 +5914,7 @@
       <c r="E66" s="12">
         <v>40488071</v>
       </c>
-      <c r="F66" s="38" t="s">
+      <c r="F66" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G66" s="12">
@@ -5941,7 +5943,7 @@
       <c r="E67" s="13">
         <v>13122266</v>
       </c>
-      <c r="F67" s="39" t="s">
+      <c r="F67" s="27" t="s">
         <v>10</v>
       </c>
       <c r="G67" s="13">
@@ -5970,7 +5972,7 @@
       <c r="E68" s="9">
         <v>407237015</v>
       </c>
-      <c r="F68" s="35" t="s">
+      <c r="F68" s="23" t="s">
         <v>10</v>
       </c>
       <c r="G68" s="9">
@@ -5999,7 +6001,7 @@
       <c r="E69" s="10">
         <v>287861188</v>
       </c>
-      <c r="F69" s="36" t="s">
+      <c r="F69" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G69" s="10">
@@ -6028,7 +6030,7 @@
       <c r="E70" s="10">
         <v>181581647</v>
       </c>
-      <c r="F70" s="36" t="s">
+      <c r="F70" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G70" s="10">
@@ -6057,7 +6059,7 @@
       <c r="E71" s="10">
         <v>174854199</v>
       </c>
-      <c r="F71" s="36" t="s">
+      <c r="F71" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G71" s="10">
@@ -6086,7 +6088,7 @@
       <c r="E72" s="10">
         <v>127015769</v>
       </c>
-      <c r="F72" s="36" t="s">
+      <c r="F72" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G72" s="10">
@@ -6115,7 +6117,7 @@
       <c r="E73" s="10">
         <v>65341846</v>
       </c>
-      <c r="F73" s="36" t="s">
+      <c r="F73" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G73" s="10">
@@ -6144,7 +6146,7 @@
       <c r="E74" s="10">
         <v>31812521</v>
       </c>
-      <c r="F74" s="36" t="s">
+      <c r="F74" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G74" s="10">
@@ -6173,7 +6175,7 @@
       <c r="E75" s="11">
         <v>444491844</v>
       </c>
-      <c r="F75" s="37" t="s">
+      <c r="F75" s="25" t="s">
         <v>10</v>
       </c>
       <c r="G75" s="11">
@@ -6202,7 +6204,7 @@
       <c r="E76" s="12">
         <v>300100866</v>
       </c>
-      <c r="F76" s="38" t="s">
+      <c r="F76" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G76" s="12">
@@ -6231,7 +6233,7 @@
       <c r="E77" s="12">
         <v>182863133</v>
       </c>
-      <c r="F77" s="38" t="s">
+      <c r="F77" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G77" s="12">
@@ -6260,7 +6262,7 @@
       <c r="E78" s="12">
         <v>171123631</v>
       </c>
-      <c r="F78" s="38" t="s">
+      <c r="F78" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G78" s="12">
@@ -6289,7 +6291,7 @@
       <c r="E79" s="12">
         <v>116988972</v>
       </c>
-      <c r="F79" s="38" t="s">
+      <c r="F79" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G79" s="12">
@@ -6318,7 +6320,7 @@
       <c r="E80" s="12">
         <v>53316617</v>
       </c>
-      <c r="F80" s="38" t="s">
+      <c r="F80" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G80" s="12">
@@ -6347,7 +6349,7 @@
       <c r="E81" s="13">
         <v>18984277</v>
       </c>
-      <c r="F81" s="39" t="s">
+      <c r="F81" s="27" t="s">
         <v>10</v>
       </c>
       <c r="G81" s="13">
@@ -6376,7 +6378,7 @@
       <c r="E82" s="9">
         <v>405869877</v>
       </c>
-      <c r="F82" s="35" t="s">
+      <c r="F82" s="23" t="s">
         <v>10</v>
       </c>
       <c r="G82" s="9">
@@ -6405,7 +6407,7 @@
       <c r="E83" s="10">
         <v>287091136</v>
       </c>
-      <c r="F83" s="36" t="s">
+      <c r="F83" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G83" s="10">
@@ -6434,7 +6436,7 @@
       <c r="E84" s="10">
         <v>179323237</v>
       </c>
-      <c r="F84" s="36" t="s">
+      <c r="F84" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G84" s="10">
@@ -6463,7 +6465,7 @@
       <c r="E85" s="10">
         <v>178643319</v>
       </c>
-      <c r="F85" s="36" t="s">
+      <c r="F85" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G85" s="10">
@@ -6492,7 +6494,7 @@
       <c r="E86" s="10">
         <v>129461666</v>
       </c>
-      <c r="F86" s="36" t="s">
+      <c r="F86" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G86" s="10">
@@ -6521,7 +6523,7 @@
       <c r="E87" s="10">
         <v>69203752</v>
       </c>
-      <c r="F87" s="36" t="s">
+      <c r="F87" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G87" s="10">
@@ -6550,7 +6552,7 @@
       <c r="E88" s="10">
         <v>32979345</v>
       </c>
-      <c r="F88" s="36" t="s">
+      <c r="F88" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G88" s="10">
@@ -6579,7 +6581,7 @@
       <c r="E89" s="11">
         <v>443023132</v>
       </c>
-      <c r="F89" s="37" t="s">
+      <c r="F89" s="25" t="s">
         <v>10</v>
       </c>
       <c r="G89" s="11">
@@ -6608,7 +6610,7 @@
       <c r="E90" s="12">
         <v>300001744</v>
       </c>
-      <c r="F90" s="38" t="s">
+      <c r="F90" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G90" s="12">
@@ -6637,7 +6639,7 @@
       <c r="E91" s="12">
         <v>180633935</v>
       </c>
-      <c r="F91" s="38" t="s">
+      <c r="F91" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G91" s="12">
@@ -6666,7 +6668,7 @@
       <c r="E92" s="12">
         <v>174836157</v>
       </c>
-      <c r="F92" s="38" t="s">
+      <c r="F92" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G92" s="12">
@@ -6695,7 +6697,7 @@
       <c r="E93" s="12">
         <v>119207503</v>
       </c>
-      <c r="F93" s="38" t="s">
+      <c r="F93" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G93" s="12">
@@ -6724,7 +6726,7 @@
       <c r="E94" s="12">
         <v>56570909</v>
       </c>
-      <c r="F94" s="38" t="s">
+      <c r="F94" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G94" s="12">
@@ -6753,7 +6755,7 @@
       <c r="E95" s="13">
         <v>19905301</v>
       </c>
-      <c r="F95" s="39" t="s">
+      <c r="F95" s="27" t="s">
         <v>10</v>
       </c>
       <c r="G95" s="13">
@@ -6782,7 +6784,7 @@
       <c r="E96" s="9">
         <v>165662419</v>
       </c>
-      <c r="F96" s="35" t="s">
+      <c r="F96" s="23" t="s">
         <v>10</v>
       </c>
       <c r="G96" s="9">
@@ -6811,7 +6813,7 @@
       <c r="E97" s="10">
         <v>117182180</v>
       </c>
-      <c r="F97" s="36" t="s">
+      <c r="F97" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G97" s="10">
@@ -6840,7 +6842,7 @@
       <c r="E98" s="10">
         <v>80201463</v>
       </c>
-      <c r="F98" s="36" t="s">
+      <c r="F98" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G98" s="10">
@@ -6869,7 +6871,7 @@
       <c r="E99" s="10">
         <v>79915749</v>
       </c>
-      <c r="F99" s="36" t="s">
+      <c r="F99" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G99" s="10">
@@ -6898,7 +6900,7 @@
       <c r="E100" s="10">
         <v>70738901</v>
       </c>
-      <c r="F100" s="36" t="s">
+      <c r="F100" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G100" s="10">
@@ -6927,7 +6929,7 @@
       <c r="E101" s="10">
         <v>52826535</v>
       </c>
-      <c r="F101" s="36" t="s">
+      <c r="F101" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G101" s="10">
@@ -6956,7 +6958,7 @@
       <c r="E102" s="10">
         <v>37916678</v>
       </c>
-      <c r="F102" s="36" t="s">
+      <c r="F102" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G102" s="10">
@@ -6985,7 +6987,7 @@
       <c r="E103" s="11">
         <v>174474243</v>
       </c>
-      <c r="F103" s="37" t="s">
+      <c r="F103" s="25" t="s">
         <v>10</v>
       </c>
       <c r="G103" s="11">
@@ -7014,7 +7016,7 @@
       <c r="E104" s="12">
         <v>127118300</v>
       </c>
-      <c r="F104" s="38" t="s">
+      <c r="F104" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G104" s="12">
@@ -7043,7 +7045,7 @@
       <c r="E105" s="12">
         <v>84245856</v>
       </c>
-      <c r="F105" s="38" t="s">
+      <c r="F105" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G105" s="12">
@@ -7072,7 +7074,7 @@
       <c r="E106" s="12">
         <v>81082010</v>
       </c>
-      <c r="F106" s="38" t="s">
+      <c r="F106" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G106" s="12">
@@ -7101,7 +7103,7 @@
       <c r="E107" s="12">
         <v>66537761</v>
       </c>
-      <c r="F107" s="38" t="s">
+      <c r="F107" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G107" s="12">
@@ -7130,7 +7132,7 @@
       <c r="E108" s="12">
         <v>44464325</v>
       </c>
-      <c r="F108" s="38" t="s">
+      <c r="F108" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G108" s="12">
@@ -7159,7 +7161,7 @@
       <c r="E109" s="13">
         <v>22955932</v>
       </c>
-      <c r="F109" s="39" t="s">
+      <c r="F109" s="27" t="s">
         <v>10</v>
       </c>
       <c r="G109" s="13">
@@ -7188,7 +7190,7 @@
       <c r="E110" s="9">
         <v>165298793</v>
       </c>
-      <c r="F110" s="35" t="s">
+      <c r="F110" s="23" t="s">
         <v>10</v>
       </c>
       <c r="G110" s="9">
@@ -7217,7 +7219,7 @@
       <c r="E111" s="10">
         <v>116774483</v>
       </c>
-      <c r="F111" s="36" t="s">
+      <c r="F111" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G111" s="10">
@@ -7246,7 +7248,7 @@
       <c r="E112" s="10">
         <v>80054907</v>
       </c>
-      <c r="F112" s="36" t="s">
+      <c r="F112" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G112" s="10">
@@ -7275,7 +7277,7 @@
       <c r="E113" s="10">
         <v>79979111</v>
       </c>
-      <c r="F113" s="36" t="s">
+      <c r="F113" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G113" s="10">
@@ -7304,7 +7306,7 @@
       <c r="E114" s="10">
         <v>71542431</v>
       </c>
-      <c r="F114" s="36" t="s">
+      <c r="F114" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G114" s="10">
@@ -7333,7 +7335,7 @@
       <c r="E115" s="10">
         <v>54109925</v>
       </c>
-      <c r="F115" s="36" t="s">
+      <c r="F115" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G115" s="10">
@@ -7362,7 +7364,7 @@
       <c r="E116" s="10">
         <v>38677425</v>
       </c>
-      <c r="F116" s="36" t="s">
+      <c r="F116" s="24" t="s">
         <v>10</v>
       </c>
       <c r="G116" s="10">
@@ -7391,7 +7393,7 @@
       <c r="E117" s="11">
         <v>174132103</v>
       </c>
-      <c r="F117" s="37" t="s">
+      <c r="F117" s="25" t="s">
         <v>10</v>
       </c>
       <c r="G117" s="11">
@@ -7420,7 +7422,7 @@
       <c r="E118" s="12">
         <v>126674018</v>
       </c>
-      <c r="F118" s="38" t="s">
+      <c r="F118" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G118" s="12">
@@ -7449,7 +7451,7 @@
       <c r="E119" s="12">
         <v>84069475</v>
       </c>
-      <c r="F119" s="38" t="s">
+      <c r="F119" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G119" s="12">
@@ -7478,7 +7480,7 @@
       <c r="E120" s="12">
         <v>81304289</v>
       </c>
-      <c r="F120" s="38" t="s">
+      <c r="F120" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G120" s="12">
@@ -7507,7 +7509,7 @@
       <c r="E121" s="12">
         <v>67527174</v>
       </c>
-      <c r="F121" s="38" t="s">
+      <c r="F121" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G121" s="12">
@@ -7536,7 +7538,7 @@
       <c r="E122" s="12">
         <v>45683675</v>
       </c>
-      <c r="F122" s="38" t="s">
+      <c r="F122" s="26" t="s">
         <v>10</v>
       </c>
       <c r="G122" s="12">
@@ -7565,7 +7567,7 @@
       <c r="E123" s="13">
         <v>23786912</v>
       </c>
-      <c r="F123" s="39" t="s">
+      <c r="F123" s="27" t="s">
         <v>10</v>
       </c>
       <c r="G123" s="13">

</xml_diff>